<commit_message>
Add Profile, Account, and Archive
</commit_message>
<xml_diff>
--- a/Data/Input/Profile-Outlook.xlsx
+++ b/Data/Input/Profile-Outlook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kampus\Semester 7\MBKM\UIPATH\Project\Archive Email\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57A44E4-11A3-494A-B1EF-2B5F5364C9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7296CEDE-34C8-40CE-9EAF-41B2FEDD1B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3045" yWindow="2280" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Profile</t>
   </si>
@@ -36,19 +36,16 @@
     <t>Account</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>Outlook Rpa</t>
   </si>
   <si>
-    <t>Outlook profile 1</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>madajabbar22@gmail.com</t>
+  </si>
+  <si>
+    <t>madajabbar@student.untan.ac.id</t>
   </si>
 </sst>
 </file>
@@ -90,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,84 +370,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>